<commit_message>
split date and time for bp excel files
</commit_message>
<xml_diff>
--- a/src/main/resources/initialDataFiles/bloodPressureReadings.xlsx
+++ b/src/main/resources/initialDataFiles/bloodPressureReadings.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catha\Documents\Health\ADHD\medTrackerInitialData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Java\SpringBootProjects\MedTracker\src\main\resources\initialDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9DC854-4A06-4BBE-AF46-431162DCF150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A8F6C18-84B5-4635-B22B-36F6B465985A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-60" windowWidth="35200" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-60" windowWidth="35200" windowHeight="21820" xr2:uid="{BE4ABE33-A413-46B3-BA4A-8E7C67A5CF00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,12 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>date</t>
+  </si>
   <si>
     <t>PrescriptionScheduleEntry</t>
-  </si>
-  <si>
-    <t>readingTime</t>
   </si>
   <si>
     <t>systole</t>
@@ -41,24 +41,21 @@
   <si>
     <t>heartRate</t>
   </si>
+  <si>
+    <t>time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ hh:mm:ss\.ss"/>
+    <numFmt numFmtId="164" formatCode="[$]hh:mm;@" x16r2:formatCode16="[$-en-NL,1]hh:mm;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,10 +81,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -122,7 +120,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -134,7 +132,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -181,6 +179,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -216,6 +231,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -367,25 +399,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129D93C5-89D8-403D-9040-DB491AF7D8F0}">
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection sqref="A1:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.453125" customWidth="1"/>
-    <col min="2" max="2" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -396,10 +427,13 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>45617.375</v>
+        <v>45623</v>
       </c>
       <c r="B2" s="2">
         <v>2</v>
@@ -413,10 +447,13 @@
       <c r="E2">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" s="3">
+        <v>0.39652777777777776</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>45617.541666666664</v>
+        <v>45624</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
@@ -430,10 +467,13 @@
       <c r="E3">
         <v>67</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" s="3">
+        <v>0.39652777777777776</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>45617.791666666664</v>
+        <v>45625</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
@@ -447,10 +487,13 @@
       <c r="E4">
         <v>68</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" s="3">
+        <v>0.39652777777777776</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>45618.375</v>
+        <v>45626</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
@@ -464,10 +507,13 @@
       <c r="E5">
         <v>69</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" s="3">
+        <v>0.43125000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>45618.541666666664</v>
+        <v>45627</v>
       </c>
       <c r="B6" s="2">
         <v>3</v>
@@ -481,10 +527,13 @@
       <c r="E6">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" s="3">
+        <v>0.41249999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>45618.791666666664</v>
+        <v>45628</v>
       </c>
       <c r="B7" s="2">
         <v>4</v>
@@ -498,10 +547,13 @@
       <c r="E7">
         <v>71</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" s="3">
+        <v>0.43055555555555558</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>45619.375</v>
+        <v>45629</v>
       </c>
       <c r="B8" s="2">
         <v>2</v>
@@ -515,10 +567,13 @@
       <c r="E8">
         <v>72</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" s="3">
+        <v>0.41249999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>45619.541666666664</v>
+        <v>45630</v>
       </c>
       <c r="B9" s="2">
         <v>3</v>
@@ -532,27 +587,11 @@
       <c r="E9">
         <v>73</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>45619.791666666664</v>
-      </c>
-      <c r="B10" s="2">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>119</v>
-      </c>
-      <c r="D10">
-        <v>85</v>
-      </c>
-      <c r="E10">
-        <v>74</v>
+      <c r="F9" s="3">
+        <v>0.40763888888888888</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
split date and time for doses.xlsx excel files
</commit_message>
<xml_diff>
--- a/src/main/resources/initialDataFiles/bloodPressureReadings.xlsx
+++ b/src/main/resources/initialDataFiles/bloodPressureReadings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Java\SpringBootProjects\MedTracker\src\main\resources\initialDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A8F6C18-84B5-4635-B22B-36F6B465985A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E898B153-4135-450D-9A20-7E83BB90A63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-60" windowWidth="35200" windowHeight="21820" xr2:uid="{BE4ABE33-A413-46B3-BA4A-8E7C67A5CF00}"/>
   </bookViews>
@@ -400,15 +400,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129D93C5-89D8-403D-9040-DB491AF7D8F0}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F9"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.36328125" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -453,145 +454,469 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>45624</v>
+        <v>45623</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
       </c>
       <c r="C3">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E3">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F3" s="3">
-        <v>0.39652777777777776</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>45625</v>
+        <v>45623</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
       </c>
       <c r="C4">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D4">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E4">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F4" s="3">
-        <v>0.39652777777777776</v>
+        <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>45626</v>
+        <v>45624</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D5">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E5">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F5" s="3">
-        <v>0.43125000000000002</v>
+        <v>0.39652777777777776</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>45627</v>
+        <v>45624</v>
       </c>
       <c r="B6" s="2">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D6">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E6">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F6" s="3">
-        <v>0.41249999999999998</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>45628</v>
+        <v>45624</v>
       </c>
       <c r="B7" s="2">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D7">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E7">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F7" s="3">
-        <v>0.43055555555555558</v>
+        <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>45629</v>
+        <v>45625</v>
       </c>
       <c r="B8" s="2">
         <v>2</v>
       </c>
       <c r="C8">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D8">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E8">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F8" s="3">
-        <v>0.41249999999999998</v>
+        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>45630</v>
+        <v>45625</v>
       </c>
       <c r="B9" s="2">
         <v>3</v>
       </c>
       <c r="C9">
+        <v>113</v>
+      </c>
+      <c r="D9">
+        <v>79</v>
+      </c>
+      <c r="E9">
+        <v>68</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.54166666666666696</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>45625</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>113</v>
+      </c>
+      <c r="D10">
+        <v>79</v>
+      </c>
+      <c r="E10">
+        <v>68</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.79166666666666696</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>45626</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>114</v>
+      </c>
+      <c r="D11">
+        <v>80</v>
+      </c>
+      <c r="E11">
+        <v>69</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>45626</v>
+      </c>
+      <c r="B12" s="2">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>114</v>
+      </c>
+      <c r="D12">
+        <v>80</v>
+      </c>
+      <c r="E12">
+        <v>69</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.54166666666666696</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>45626</v>
+      </c>
+      <c r="B13" s="2">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>114</v>
+      </c>
+      <c r="D13">
+        <v>80</v>
+      </c>
+      <c r="E13">
+        <v>69</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.79166666666666696</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>45627</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>115</v>
+      </c>
+      <c r="D14">
+        <v>81</v>
+      </c>
+      <c r="E14">
+        <v>70</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>45627</v>
+      </c>
+      <c r="B15" s="2">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>115</v>
+      </c>
+      <c r="D15">
+        <v>81</v>
+      </c>
+      <c r="E15">
+        <v>70</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.54166666666666696</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>45627</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>115</v>
+      </c>
+      <c r="D16">
+        <v>81</v>
+      </c>
+      <c r="E16">
+        <v>70</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.79166666666666696</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>45628</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>116</v>
+      </c>
+      <c r="D17">
+        <v>82</v>
+      </c>
+      <c r="E17">
+        <v>71</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>45628</v>
+      </c>
+      <c r="B18" s="2">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>116</v>
+      </c>
+      <c r="D18">
+        <v>82</v>
+      </c>
+      <c r="E18">
+        <v>71</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.54166666666666696</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>45628</v>
+      </c>
+      <c r="B19" s="2">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>116</v>
+      </c>
+      <c r="D19">
+        <v>82</v>
+      </c>
+      <c r="E19">
+        <v>71</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.79166666666666696</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>45629</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>117</v>
+      </c>
+      <c r="D20">
+        <v>83</v>
+      </c>
+      <c r="E20">
+        <v>72</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>45629</v>
+      </c>
+      <c r="B21" s="2">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>117</v>
+      </c>
+      <c r="D21">
+        <v>83</v>
+      </c>
+      <c r="E21">
+        <v>72</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.54166666666666696</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>45629</v>
+      </c>
+      <c r="B22" s="2">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>117</v>
+      </c>
+      <c r="D22">
+        <v>83</v>
+      </c>
+      <c r="E22">
+        <v>72</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.79166666666666696</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>45630</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2</v>
+      </c>
+      <c r="C23">
         <v>118</v>
       </c>
-      <c r="D9">
+      <c r="D23">
         <v>84</v>
       </c>
-      <c r="E9">
+      <c r="E23">
         <v>73</v>
       </c>
-      <c r="F9" s="3">
-        <v>0.40763888888888888</v>
+      <c r="F23" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>45630</v>
+      </c>
+      <c r="B24" s="2">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>118</v>
+      </c>
+      <c r="D24">
+        <v>84</v>
+      </c>
+      <c r="E24">
+        <v>73</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0.54166666666666696</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>45630</v>
+      </c>
+      <c r="B25" s="2">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>118</v>
+      </c>
+      <c r="D25">
+        <v>84</v>
+      </c>
+      <c r="E25">
+        <v>73</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0.79166666666666696</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F25">
+    <sortCondition ref="A2:A25"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BloodPressureReading should refer to a DAYSTAGE not a prescriptionScheduleEntry, fixed upload and initial data to  reflect this.
</commit_message>
<xml_diff>
--- a/src/main/resources/initialDataFiles/bloodPressureReadings.xlsx
+++ b/src/main/resources/initialDataFiles/bloodPressureReadings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Java\SpringBootProjects\MedTracker\src\main\resources\initialDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E898B153-4135-450D-9A20-7E83BB90A63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174402FA-2C88-45AC-9D64-5C3CE6FC6A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-60" windowWidth="35200" windowHeight="21820" xr2:uid="{BE4ABE33-A413-46B3-BA4A-8E7C67A5CF00}"/>
+    <workbookView xWindow="-32750" yWindow="2590" windowWidth="26460" windowHeight="15910" xr2:uid="{BE4ABE33-A413-46B3-BA4A-8E7C67A5CF00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="9">
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>PrescriptionScheduleEntry</t>
   </si>
   <si>
     <t>systole</t>
@@ -43,6 +40,18 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>dayStage</t>
+  </si>
+  <si>
+    <t>MORNING</t>
+  </si>
+  <si>
+    <t>AFTERNOON</t>
+  </si>
+  <si>
+    <t>MIDDAY</t>
   </si>
 </sst>
 </file>
@@ -403,13 +412,13 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="B2" sqref="B2:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.36328125" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -417,27 +426,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45623</v>
       </c>
-      <c r="B2" s="2">
-        <v>2</v>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C2">
         <v>111</v>
@@ -456,8 +465,8 @@
       <c r="A3" s="1">
         <v>45623</v>
       </c>
-      <c r="B3" s="2">
-        <v>3</v>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C3">
         <v>111</v>
@@ -476,8 +485,8 @@
       <c r="A4" s="1">
         <v>45623</v>
       </c>
-      <c r="B4" s="2">
-        <v>4</v>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C4">
         <v>111</v>
@@ -496,8 +505,8 @@
       <c r="A5" s="1">
         <v>45624</v>
       </c>
-      <c r="B5" s="2">
-        <v>2</v>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C5">
         <v>112</v>
@@ -516,8 +525,8 @@
       <c r="A6" s="1">
         <v>45624</v>
       </c>
-      <c r="B6" s="2">
-        <v>3</v>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C6">
         <v>112</v>
@@ -536,8 +545,8 @@
       <c r="A7" s="1">
         <v>45624</v>
       </c>
-      <c r="B7" s="2">
-        <v>4</v>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C7">
         <v>112</v>
@@ -556,8 +565,8 @@
       <c r="A8" s="1">
         <v>45625</v>
       </c>
-      <c r="B8" s="2">
-        <v>2</v>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C8">
         <v>113</v>
@@ -576,8 +585,8 @@
       <c r="A9" s="1">
         <v>45625</v>
       </c>
-      <c r="B9" s="2">
-        <v>3</v>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C9">
         <v>113</v>
@@ -596,8 +605,8 @@
       <c r="A10" s="1">
         <v>45625</v>
       </c>
-      <c r="B10" s="2">
-        <v>4</v>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C10">
         <v>113</v>
@@ -616,8 +625,8 @@
       <c r="A11" s="1">
         <v>45626</v>
       </c>
-      <c r="B11" s="2">
-        <v>2</v>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C11">
         <v>114</v>
@@ -636,8 +645,8 @@
       <c r="A12" s="1">
         <v>45626</v>
       </c>
-      <c r="B12" s="2">
-        <v>3</v>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C12">
         <v>114</v>
@@ -656,8 +665,8 @@
       <c r="A13" s="1">
         <v>45626</v>
       </c>
-      <c r="B13" s="2">
-        <v>4</v>
+      <c r="B13" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C13">
         <v>114</v>
@@ -676,8 +685,8 @@
       <c r="A14" s="1">
         <v>45627</v>
       </c>
-      <c r="B14" s="2">
-        <v>2</v>
+      <c r="B14" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C14">
         <v>115</v>
@@ -696,8 +705,8 @@
       <c r="A15" s="1">
         <v>45627</v>
       </c>
-      <c r="B15" s="2">
-        <v>3</v>
+      <c r="B15" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C15">
         <v>115</v>
@@ -716,8 +725,8 @@
       <c r="A16" s="1">
         <v>45627</v>
       </c>
-      <c r="B16" s="2">
-        <v>4</v>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C16">
         <v>115</v>
@@ -736,8 +745,8 @@
       <c r="A17" s="1">
         <v>45628</v>
       </c>
-      <c r="B17" s="2">
-        <v>2</v>
+      <c r="B17" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C17">
         <v>116</v>
@@ -756,8 +765,8 @@
       <c r="A18" s="1">
         <v>45628</v>
       </c>
-      <c r="B18" s="2">
-        <v>3</v>
+      <c r="B18" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C18">
         <v>116</v>
@@ -776,8 +785,8 @@
       <c r="A19" s="1">
         <v>45628</v>
       </c>
-      <c r="B19" s="2">
-        <v>4</v>
+      <c r="B19" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C19">
         <v>116</v>
@@ -796,8 +805,8 @@
       <c r="A20" s="1">
         <v>45629</v>
       </c>
-      <c r="B20" s="2">
-        <v>2</v>
+      <c r="B20" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C20">
         <v>117</v>
@@ -816,8 +825,8 @@
       <c r="A21" s="1">
         <v>45629</v>
       </c>
-      <c r="B21" s="2">
-        <v>3</v>
+      <c r="B21" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C21">
         <v>117</v>
@@ -836,8 +845,8 @@
       <c r="A22" s="1">
         <v>45629</v>
       </c>
-      <c r="B22" s="2">
-        <v>4</v>
+      <c r="B22" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C22">
         <v>117</v>
@@ -856,8 +865,8 @@
       <c r="A23" s="1">
         <v>45630</v>
       </c>
-      <c r="B23" s="2">
-        <v>2</v>
+      <c r="B23" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C23">
         <v>118</v>
@@ -876,8 +885,8 @@
       <c r="A24" s="1">
         <v>45630</v>
       </c>
-      <c r="B24" s="2">
-        <v>3</v>
+      <c r="B24" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C24">
         <v>118</v>
@@ -896,8 +905,8 @@
       <c r="A25" s="1">
         <v>45630</v>
       </c>
-      <c r="B25" s="2">
-        <v>4</v>
+      <c r="B25" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C25">
         <v>118</v>

</xml_diff>

<commit_message>
filter out empty BloodPressureReading during uploads. added more complex initial data files
</commit_message>
<xml_diff>
--- a/src/main/resources/initialDataFiles/bloodPressureReadings.xlsx
+++ b/src/main/resources/initialDataFiles/bloodPressureReadings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Java\SpringBootProjects\MedTracker\src\main\resources\initialDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174402FA-2C88-45AC-9D64-5C3CE6FC6A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E58CB24-22DD-4005-923B-E0F87F266A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32750" yWindow="2590" windowWidth="26460" windowHeight="15910" xr2:uid="{BE4ABE33-A413-46B3-BA4A-8E7C67A5CF00}"/>
+    <workbookView xWindow="-38510" yWindow="-60" windowWidth="35200" windowHeight="21820" xr2:uid="{BE4ABE33-A413-46B3-BA4A-8E7C67A5CF00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="10">
   <si>
     <t>date</t>
   </si>
@@ -53,6 +53,9 @@
   <si>
     <t>MIDDAY</t>
   </si>
+  <si>
+    <t>EVENING</t>
+  </si>
 </sst>
 </file>
 
@@ -61,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$]hh:mm;@" x16r2:formatCode16="[$-en-NL,1]hh:mm;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,13 +72,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -87,16 +114,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129D93C5-89D8-403D-9040-DB491AF7D8F0}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B25"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92:F93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -443,79 +476,79 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>45623</v>
+        <v>45582</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D2">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E2">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F2" s="3">
-        <v>0.39652777777777776</v>
+        <v>0.76875000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>45623</v>
+        <v>45583</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D3">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E3">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F3" s="3">
-        <v>0.54166666666666663</v>
+        <v>0.39652777777777776</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>45623</v>
+        <v>45584</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="D4">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E4">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F4" s="3">
-        <v>0.79166666666666663</v>
+        <v>0.39652777777777776</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>45624</v>
+        <v>45585</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="D5">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E5">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F5" s="3">
         <v>0.39652777777777776</v>
@@ -523,59 +556,59 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>45624</v>
+        <v>45586</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D6">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E6">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="F6" s="3">
-        <v>0.54166666666666663</v>
+        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>45624</v>
+        <v>45587</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="D7">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E7">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F7" s="3">
-        <v>0.79166666666666663</v>
+        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>45625</v>
+        <v>45588</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C8">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="D8">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E8">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F8" s="3">
         <v>0.39652777777777798</v>
@@ -583,59 +616,59 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>45625</v>
+        <v>45589</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="D9">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E9">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F9" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>45625</v>
+        <v>45590</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="D10">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E10">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F10" s="3">
-        <v>0.79166666666666696</v>
+        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>45626</v>
+        <v>45591</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C11">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="D11">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E11">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F11" s="3">
         <v>0.39652777777777798</v>
@@ -643,59 +676,59 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>45626</v>
+        <v>45592</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="D12">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E12">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F12" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>45626</v>
+        <v>45593</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="D13">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E13">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F13" s="3">
-        <v>0.79166666666666696</v>
+        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>45627</v>
+        <v>45594</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C14">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="D14">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E14">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F14" s="3">
         <v>0.39652777777777798</v>
@@ -703,56 +736,56 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>45627</v>
+        <v>45595</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="D15">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E15">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F15" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>45627</v>
+        <v>45596</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="D16">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E16">
         <v>70</v>
       </c>
       <c r="F16" s="3">
-        <v>0.79166666666666696</v>
+        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>45628</v>
+        <v>45597</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C17">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="D17">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E17">
         <v>71</v>
@@ -763,167 +796,1527 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>45628</v>
+        <v>45598</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C18">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="D18">
         <v>82</v>
       </c>
       <c r="E18">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F18" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>45628</v>
+        <v>45599</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="D19">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E19">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F19" s="3">
-        <v>0.79166666666666696</v>
+        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>45629</v>
+        <v>45599</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C20">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="D20">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E20">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F20" s="3">
-        <v>0.39652777777777798</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>45629</v>
+        <v>45599</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="D21">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E21">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F21" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>45629</v>
+        <v>45600</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="D22">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E22">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F22" s="3">
-        <v>0.79166666666666696</v>
+        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>45630</v>
+        <v>45600</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C23">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="D23">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E23">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F23" s="3">
-        <v>0.39652777777777798</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>45630</v>
+        <v>45600</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="D24">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E24">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F24" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>45630</v>
+        <v>45601</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>139</v>
+      </c>
+      <c r="D25">
+        <v>89</v>
+      </c>
+      <c r="E25">
+        <v>79</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>45601</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>140</v>
+      </c>
+      <c r="D26">
+        <v>90</v>
+      </c>
+      <c r="E26">
+        <v>80</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>45601</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C25">
+      <c r="C27">
+        <v>114</v>
+      </c>
+      <c r="D27">
+        <v>91</v>
+      </c>
+      <c r="E27">
+        <v>81</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>45602</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28">
+        <v>112</v>
+      </c>
+      <c r="D28">
+        <v>92</v>
+      </c>
+      <c r="E28">
+        <v>82</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>45602</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>110</v>
+      </c>
+      <c r="D29">
+        <v>93</v>
+      </c>
+      <c r="E29">
+        <v>83</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>45602</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>108</v>
+      </c>
+      <c r="D30">
+        <v>94</v>
+      </c>
+      <c r="E30">
+        <v>84</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>45603</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>106</v>
+      </c>
+      <c r="D31">
+        <v>95</v>
+      </c>
+      <c r="E31">
+        <v>85</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>45603</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>104</v>
+      </c>
+      <c r="D32">
+        <v>96</v>
+      </c>
+      <c r="E32">
+        <v>86</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>45603</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>102</v>
+      </c>
+      <c r="D33">
+        <v>97</v>
+      </c>
+      <c r="E33">
+        <v>87</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>45604</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34">
+        <v>100</v>
+      </c>
+      <c r="D34">
+        <v>98</v>
+      </c>
+      <c r="E34">
+        <v>88</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>45604</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>98</v>
+      </c>
+      <c r="D35">
+        <v>99</v>
+      </c>
+      <c r="E35">
+        <v>89</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>45604</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>96</v>
+      </c>
+      <c r="D36">
+        <v>100</v>
+      </c>
+      <c r="E36">
+        <v>69</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>45605</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="5">
+        <v>146</v>
+      </c>
+      <c r="D37">
+        <v>101</v>
+      </c>
+      <c r="E37">
+        <v>65</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>45605</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="5">
+        <v>132</v>
+      </c>
+      <c r="D38">
+        <v>102</v>
+      </c>
+      <c r="E38">
+        <v>71</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>45605</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="5">
+        <v>138</v>
+      </c>
+      <c r="D39">
+        <v>77</v>
+      </c>
+      <c r="E39">
+        <v>77</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <v>45606</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40">
+        <v>125</v>
+      </c>
+      <c r="D40">
+        <v>81</v>
+      </c>
+      <c r="E40">
+        <v>83</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="1">
+        <v>45606</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="4">
+        <v>127</v>
+      </c>
+      <c r="D41">
+        <v>85</v>
+      </c>
+      <c r="E41">
+        <v>89</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
+        <v>45607</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42">
+        <v>129</v>
+      </c>
+      <c r="D42">
+        <v>89</v>
+      </c>
+      <c r="E42">
+        <v>95</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="1">
+        <v>45607</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="4">
+        <v>131</v>
+      </c>
+      <c r="D43">
+        <v>93</v>
+      </c>
+      <c r="E43">
+        <v>101</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="1">
+        <v>45607</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44">
+        <v>133</v>
+      </c>
+      <c r="D44">
+        <v>97</v>
+      </c>
+      <c r="E44">
+        <v>77</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="1">
+        <v>45608</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="4">
+        <v>135</v>
+      </c>
+      <c r="D45">
+        <v>101</v>
+      </c>
+      <c r="E45">
+        <v>74</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="1">
+        <v>45608</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46">
+        <v>137</v>
+      </c>
+      <c r="D46">
+        <v>105</v>
+      </c>
+      <c r="E46">
+        <v>75</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="1">
+        <v>45608</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="4">
+        <v>139</v>
+      </c>
+      <c r="D47">
+        <v>75</v>
+      </c>
+      <c r="E47">
+        <v>76</v>
+      </c>
+      <c r="F47" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="1">
+        <v>45609</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48">
+        <v>141</v>
+      </c>
+      <c r="D48">
+        <v>73</v>
+      </c>
+      <c r="E48">
+        <v>77</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>45609</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="4">
+        <v>143</v>
+      </c>
+      <c r="D49" s="2">
+        <v>70</v>
+      </c>
+      <c r="E49">
+        <v>78</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>45609</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50">
+        <v>145</v>
+      </c>
+      <c r="D50">
+        <v>74</v>
+      </c>
+      <c r="E50">
+        <v>79</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>45610</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="4">
+        <v>147</v>
+      </c>
+      <c r="D51">
+        <v>75</v>
+      </c>
+      <c r="E51">
+        <v>80</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>45610</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52">
+        <v>108</v>
+      </c>
+      <c r="D52">
+        <v>76</v>
+      </c>
+      <c r="E52">
+        <v>81</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>45610</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53">
+        <v>107</v>
+      </c>
+      <c r="D53">
+        <v>77</v>
+      </c>
+      <c r="E53">
+        <v>82</v>
+      </c>
+      <c r="F53" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="1">
+        <v>45611</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54">
+        <v>106</v>
+      </c>
+      <c r="D54">
+        <v>78</v>
+      </c>
+      <c r="E54">
+        <v>83</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" s="1">
+        <v>45611</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55">
+        <v>105</v>
+      </c>
+      <c r="D55">
+        <v>79</v>
+      </c>
+      <c r="E55">
+        <v>84</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" s="1">
+        <v>45611</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56">
+        <v>104</v>
+      </c>
+      <c r="D56">
+        <v>80</v>
+      </c>
+      <c r="E56">
+        <v>85</v>
+      </c>
+      <c r="F56" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" s="1">
+        <v>45612</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57">
+        <v>103</v>
+      </c>
+      <c r="D57">
+        <v>81</v>
+      </c>
+      <c r="E57">
+        <v>86</v>
+      </c>
+      <c r="F57" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" s="1">
+        <v>45612</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>102</v>
+      </c>
+      <c r="D58">
+        <v>82</v>
+      </c>
+      <c r="E58">
+        <v>87</v>
+      </c>
+      <c r="F58" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" s="1">
+        <v>45612</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59">
+        <v>101</v>
+      </c>
+      <c r="D59">
+        <v>83</v>
+      </c>
+      <c r="E59">
+        <v>88</v>
+      </c>
+      <c r="F59" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" s="1">
+        <v>45613</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60">
+        <v>121</v>
+      </c>
+      <c r="D60">
+        <v>84</v>
+      </c>
+      <c r="E60">
+        <v>89</v>
+      </c>
+      <c r="F60" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" s="1">
+        <v>45613</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61">
+        <v>121</v>
+      </c>
+      <c r="D61">
+        <v>85</v>
+      </c>
+      <c r="E61">
+        <v>90</v>
+      </c>
+      <c r="F61" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" s="1">
+        <v>45613</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62">
+        <v>121</v>
+      </c>
+      <c r="D62">
+        <v>86</v>
+      </c>
+      <c r="E62">
+        <v>91</v>
+      </c>
+      <c r="F62" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" s="1">
+        <v>45614</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63">
+        <v>121</v>
+      </c>
+      <c r="D63">
+        <v>87</v>
+      </c>
+      <c r="E63">
+        <v>92</v>
+      </c>
+      <c r="F63" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64" s="1">
+        <v>45614</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64">
+        <v>120</v>
+      </c>
+      <c r="D64">
+        <v>88</v>
+      </c>
+      <c r="E64">
+        <v>93</v>
+      </c>
+      <c r="F64" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65" s="1">
+        <v>45614</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65">
+        <v>120</v>
+      </c>
+      <c r="D65">
+        <v>89</v>
+      </c>
+      <c r="E65">
+        <v>94</v>
+      </c>
+      <c r="F65" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66" s="1">
+        <v>45615</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66">
+        <v>120</v>
+      </c>
+      <c r="D66">
+        <v>90</v>
+      </c>
+      <c r="E66">
+        <v>82</v>
+      </c>
+      <c r="F66" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" s="1">
+        <v>45615</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67">
+        <v>120</v>
+      </c>
+      <c r="D67">
+        <v>91</v>
+      </c>
+      <c r="E67">
+        <v>71</v>
+      </c>
+      <c r="F67" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68" s="1">
+        <v>45615</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68">
+        <v>120</v>
+      </c>
+      <c r="D68">
+        <v>92</v>
+      </c>
+      <c r="E68">
+        <v>57</v>
+      </c>
+      <c r="F68" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69" s="1">
+        <v>45616</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69">
+        <v>120</v>
+      </c>
+      <c r="D69">
+        <v>93</v>
+      </c>
+      <c r="E69">
+        <v>76</v>
+      </c>
+      <c r="F69" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" s="1">
+        <v>45616</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70">
+        <v>120</v>
+      </c>
+      <c r="D70">
+        <v>94</v>
+      </c>
+      <c r="E70">
+        <v>65</v>
+      </c>
+      <c r="F70" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71" s="1">
+        <v>45616</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71">
+        <v>120</v>
+      </c>
+      <c r="D71">
+        <v>95</v>
+      </c>
+      <c r="E71">
+        <v>65</v>
+      </c>
+      <c r="F71" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72" s="1">
+        <v>45617</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72">
+        <v>120</v>
+      </c>
+      <c r="D72">
+        <v>96</v>
+      </c>
+      <c r="E72">
+        <v>67</v>
+      </c>
+      <c r="F72" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A73" s="1">
+        <v>45617</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73">
+        <v>120</v>
+      </c>
+      <c r="D73">
+        <v>97</v>
+      </c>
+      <c r="E73">
+        <v>69</v>
+      </c>
+      <c r="F73" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A74" s="1">
+        <v>45618</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C74">
+        <v>120</v>
+      </c>
+      <c r="D74">
+        <v>98</v>
+      </c>
+      <c r="E74">
+        <v>71</v>
+      </c>
+      <c r="F74" s="3">
+        <v>0.41944444444444445</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A75" s="1">
+        <v>45618</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75">
+        <v>111</v>
+      </c>
+      <c r="D75">
+        <v>99</v>
+      </c>
+      <c r="E75">
+        <v>73</v>
+      </c>
+      <c r="F75" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A76" s="1">
+        <v>45618</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76">
+        <v>111</v>
+      </c>
+      <c r="D76">
+        <v>100</v>
+      </c>
+      <c r="E76">
+        <v>75</v>
+      </c>
+      <c r="F76" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A77" s="1">
+        <v>45619</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77">
         <v>118</v>
       </c>
-      <c r="D25">
-        <v>84</v>
-      </c>
-      <c r="E25">
-        <v>73</v>
-      </c>
-      <c r="F25" s="3">
-        <v>0.79166666666666696</v>
+      <c r="D77">
+        <v>101</v>
+      </c>
+      <c r="E77">
+        <v>77</v>
+      </c>
+      <c r="F77" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A78" s="1">
+        <v>45620</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78">
+        <v>108</v>
+      </c>
+      <c r="D78">
+        <v>102</v>
+      </c>
+      <c r="E78">
+        <v>79</v>
+      </c>
+      <c r="F78" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A79" s="1">
+        <v>45620</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79">
+        <v>117</v>
+      </c>
+      <c r="D79" s="2">
+        <v>72</v>
+      </c>
+      <c r="E79">
+        <v>81</v>
+      </c>
+      <c r="F79" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A80" s="1">
+        <v>45620</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80">
+        <v>126</v>
+      </c>
+      <c r="D80" s="2">
+        <v>72</v>
+      </c>
+      <c r="E80">
+        <v>83</v>
+      </c>
+      <c r="F80" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A81" s="1">
+        <v>45621</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81">
+        <v>117</v>
+      </c>
+      <c r="D81" s="2">
+        <v>72</v>
+      </c>
+      <c r="E81">
+        <v>85</v>
+      </c>
+      <c r="F81" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A82" s="1">
+        <v>45621</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82">
+        <v>119</v>
+      </c>
+      <c r="D82" s="2">
+        <v>72</v>
+      </c>
+      <c r="E82">
+        <v>87</v>
+      </c>
+      <c r="F82" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A83" s="1">
+        <v>45621</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C83">
+        <v>117</v>
+      </c>
+      <c r="D83" s="2">
+        <v>72</v>
+      </c>
+      <c r="E83">
+        <v>89</v>
+      </c>
+      <c r="F83" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A84" s="1">
+        <v>45622</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84">
+        <v>118</v>
+      </c>
+      <c r="D84">
+        <v>75</v>
+      </c>
+      <c r="E84">
+        <v>91</v>
+      </c>
+      <c r="F84" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A85" s="1">
+        <v>45622</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85">
+        <v>119</v>
+      </c>
+      <c r="D85" s="2">
+        <v>75</v>
+      </c>
+      <c r="E85">
+        <v>75</v>
+      </c>
+      <c r="F85" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A86" s="1">
+        <v>45622</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86">
+        <v>120</v>
+      </c>
+      <c r="D86">
+        <v>75</v>
+      </c>
+      <c r="E86">
+        <v>64</v>
+      </c>
+      <c r="F86" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A87" s="1">
+        <v>45623</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87">
+        <v>121</v>
+      </c>
+      <c r="D87">
+        <v>76</v>
+      </c>
+      <c r="E87">
+        <v>60</v>
+      </c>
+      <c r="F87" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A88" s="1">
+        <v>45623</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88">
+        <v>122</v>
+      </c>
+      <c r="D88">
+        <v>77</v>
+      </c>
+      <c r="E88">
+        <v>61</v>
+      </c>
+      <c r="F88" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A89" s="1">
+        <v>45623</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C89">
+        <v>123</v>
+      </c>
+      <c r="D89">
+        <v>78</v>
+      </c>
+      <c r="E89">
+        <v>61</v>
+      </c>
+      <c r="F89" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A90" s="1">
+        <v>45624</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90">
+        <v>124</v>
+      </c>
+      <c r="D90">
+        <v>79</v>
+      </c>
+      <c r="E90">
+        <v>61</v>
+      </c>
+      <c r="F90" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A91" s="1">
+        <v>45624</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91">
+        <v>125</v>
+      </c>
+      <c r="D91">
+        <v>80</v>
+      </c>
+      <c r="E91">
+        <v>61</v>
+      </c>
+      <c r="F91" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A92" s="1">
+        <v>45625</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C92">
+        <v>126</v>
+      </c>
+      <c r="D92">
+        <v>81</v>
+      </c>
+      <c r="E92">
+        <v>61</v>
+      </c>
+      <c r="F92" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A93" s="1">
+        <v>45625</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C93">
+        <v>127</v>
+      </c>
+      <c r="D93">
+        <v>82</v>
+      </c>
+      <c r="E93">
+        <v>61</v>
+      </c>
+      <c r="F93" s="3">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F25">
-    <sortCondition ref="A2:A25"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F93">
+    <sortCondition ref="A2:A93"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
moved time column to 3rd position and updated importer
</commit_message>
<xml_diff>
--- a/src/main/resources/initialDataFiles/bloodPressureReadings.xlsx
+++ b/src/main/resources/initialDataFiles/bloodPressureReadings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Java\SpringBootProjects\MedTracker\src\main\resources\initialDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E58CB24-22DD-4005-923B-E0F87F266A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2919C7D-EDF2-4508-915D-0DED862492E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-60" windowWidth="35200" windowHeight="21820" xr2:uid="{BE4ABE33-A413-46B3-BA4A-8E7C67A5CF00}"/>
   </bookViews>
@@ -444,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129D93C5-89D8-403D-9040-DB491AF7D8F0}">
   <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92:F93"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -462,16 +462,16 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -481,17 +481,17 @@
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
+        <v>0.76875000000000004</v>
+      </c>
+      <c r="D2">
         <v>116</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>71</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>58</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0.76875000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -501,17 +501,17 @@
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
+        <v>0.39652777777777776</v>
+      </c>
+      <c r="D3">
         <v>117</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>67</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>59</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0.39652777777777776</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -521,17 +521,17 @@
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
+        <v>0.39652777777777776</v>
+      </c>
+      <c r="D4">
         <v>118</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>68</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>59</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0.39652777777777776</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -541,17 +541,17 @@
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
+        <v>0.39652777777777776</v>
+      </c>
+      <c r="D5">
         <v>119</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>69</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>59</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.39652777777777776</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -561,17 +561,17 @@
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D6">
         <v>120</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>70</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>55</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -581,17 +581,17 @@
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D7">
         <v>121</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>71</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>61</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -601,17 +601,17 @@
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D8">
         <v>122</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>72</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>62</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -621,17 +621,17 @@
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D9">
         <v>123</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>73</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>63</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -641,17 +641,17 @@
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D10">
         <v>124</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>74</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>64</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -661,17 +661,17 @@
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D11">
         <v>125</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>75</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>65</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -681,17 +681,17 @@
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D12">
         <v>126</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>76</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>66</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -701,17 +701,17 @@
       <c r="B13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D13">
         <v>127</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>77</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>67</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -721,17 +721,17 @@
       <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D14">
         <v>128</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>78</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>68</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -741,17 +741,17 @@
       <c r="B15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D15">
         <v>129</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>79</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>69</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -761,17 +761,17 @@
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D16">
         <v>130</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>80</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>70</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -781,17 +781,17 @@
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D17">
         <v>131</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>81</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>71</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -801,17 +801,17 @@
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D18">
         <v>132</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>82</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>72</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -821,17 +821,17 @@
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D19">
         <v>133</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>83</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>73</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -841,17 +841,17 @@
       <c r="B20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D20">
         <v>134</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>84</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>74</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -861,17 +861,17 @@
       <c r="B21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D21">
         <v>135</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>85</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>75</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -881,17 +881,17 @@
       <c r="B22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D22">
         <v>136</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>86</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>76</v>
-      </c>
-      <c r="F22" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -901,17 +901,17 @@
       <c r="B23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D23">
         <v>137</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>87</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>77</v>
-      </c>
-      <c r="F23" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -921,17 +921,17 @@
       <c r="B24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D24">
         <v>138</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>88</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>78</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -941,17 +941,17 @@
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D25">
         <v>139</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>89</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>79</v>
-      </c>
-      <c r="F25" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -961,17 +961,17 @@
       <c r="B26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D26">
         <v>140</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>90</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>80</v>
-      </c>
-      <c r="F26" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -981,17 +981,17 @@
       <c r="B27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D27">
         <v>114</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>91</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>81</v>
-      </c>
-      <c r="F27" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -1001,17 +1001,17 @@
       <c r="B28" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D28">
         <v>112</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>92</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>82</v>
-      </c>
-      <c r="F28" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -1021,17 +1021,17 @@
       <c r="B29" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D29">
         <v>110</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>93</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>83</v>
-      </c>
-      <c r="F29" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -1041,17 +1041,17 @@
       <c r="B30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D30">
         <v>108</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>94</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>84</v>
-      </c>
-      <c r="F30" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -1061,17 +1061,17 @@
       <c r="B31" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D31">
         <v>106</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>95</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>85</v>
-      </c>
-      <c r="F31" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -1081,17 +1081,17 @@
       <c r="B32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D32">
         <v>104</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>96</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>86</v>
-      </c>
-      <c r="F32" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -1101,17 +1101,17 @@
       <c r="B33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D33">
         <v>102</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>97</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>87</v>
-      </c>
-      <c r="F33" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1121,17 +1121,17 @@
       <c r="B34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D34">
         <v>100</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>98</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>88</v>
-      </c>
-      <c r="F34" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -1141,17 +1141,17 @@
       <c r="B35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D35">
         <v>98</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>99</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>89</v>
-      </c>
-      <c r="F35" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -1161,17 +1161,17 @@
       <c r="B36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D36">
         <v>96</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>100</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>69</v>
-      </c>
-      <c r="F36" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -1181,17 +1181,17 @@
       <c r="B37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D37" s="5">
         <v>146</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>101</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>65</v>
-      </c>
-      <c r="F37" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -1201,17 +1201,17 @@
       <c r="B38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D38" s="5">
         <v>132</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>102</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>71</v>
-      </c>
-      <c r="F38" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -1221,17 +1221,17 @@
       <c r="B39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D39" s="5">
         <v>138</v>
-      </c>
-      <c r="D39">
-        <v>77</v>
       </c>
       <c r="E39">
         <v>77</v>
       </c>
-      <c r="F39" s="3">
-        <v>0.66666666666666663</v>
+      <c r="F39">
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -1241,17 +1241,17 @@
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D40">
         <v>125</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>81</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>83</v>
-      </c>
-      <c r="F40" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -1261,17 +1261,17 @@
       <c r="B41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D41" s="4">
         <v>127</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>85</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>89</v>
-      </c>
-      <c r="F41" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -1281,17 +1281,17 @@
       <c r="B42" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D42">
         <v>129</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>89</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>95</v>
-      </c>
-      <c r="F42" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -1301,17 +1301,17 @@
       <c r="B43" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D43" s="4">
         <v>131</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>93</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>101</v>
-      </c>
-      <c r="F43" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -1321,17 +1321,17 @@
       <c r="B44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D44">
         <v>133</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>97</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>77</v>
-      </c>
-      <c r="F44" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
@@ -1341,17 +1341,17 @@
       <c r="B45" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D45" s="4">
         <v>135</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>101</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>74</v>
-      </c>
-      <c r="F45" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
@@ -1361,17 +1361,17 @@
       <c r="B46" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D46">
         <v>137</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>105</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>75</v>
-      </c>
-      <c r="F46" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
@@ -1381,17 +1381,17 @@
       <c r="B47" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C47" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D47" s="4">
         <v>139</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>75</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>76</v>
-      </c>
-      <c r="F47" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
@@ -1401,17 +1401,17 @@
       <c r="B48" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D48">
         <v>141</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>73</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>77</v>
-      </c>
-      <c r="F48" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -1421,17 +1421,17 @@
       <c r="B49" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D49" s="4">
         <v>143</v>
       </c>
-      <c r="D49" s="2">
+      <c r="E49" s="2">
         <v>70</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>78</v>
-      </c>
-      <c r="F49" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -1441,17 +1441,17 @@
       <c r="B50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D50">
         <v>145</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <v>74</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>79</v>
-      </c>
-      <c r="F50" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
@@ -1461,17 +1461,17 @@
       <c r="B51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C51" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D51" s="4">
         <v>147</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>75</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>80</v>
-      </c>
-      <c r="F51" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
@@ -1481,17 +1481,17 @@
       <c r="B52" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D52">
         <v>108</v>
       </c>
-      <c r="D52">
+      <c r="E52">
         <v>76</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>81</v>
-      </c>
-      <c r="F52" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
@@ -1501,17 +1501,17 @@
       <c r="B53" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D53">
         <v>107</v>
       </c>
-      <c r="D53">
+      <c r="E53">
         <v>77</v>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>82</v>
-      </c>
-      <c r="F53" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
@@ -1521,17 +1521,17 @@
       <c r="B54" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D54">
         <v>106</v>
       </c>
-      <c r="D54">
+      <c r="E54">
         <v>78</v>
       </c>
-      <c r="E54">
+      <c r="F54">
         <v>83</v>
-      </c>
-      <c r="F54" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
@@ -1541,17 +1541,17 @@
       <c r="B55" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D55">
         <v>105</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <v>79</v>
       </c>
-      <c r="E55">
+      <c r="F55">
         <v>84</v>
-      </c>
-      <c r="F55" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
@@ -1561,17 +1561,17 @@
       <c r="B56" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D56">
         <v>104</v>
       </c>
-      <c r="D56">
+      <c r="E56">
         <v>80</v>
       </c>
-      <c r="E56">
+      <c r="F56">
         <v>85</v>
-      </c>
-      <c r="F56" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
@@ -1581,17 +1581,17 @@
       <c r="B57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D57">
         <v>103</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>81</v>
       </c>
-      <c r="E57">
+      <c r="F57">
         <v>86</v>
-      </c>
-      <c r="F57" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -1601,17 +1601,17 @@
       <c r="B58" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D58">
         <v>102</v>
       </c>
-      <c r="D58">
+      <c r="E58">
         <v>82</v>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>87</v>
-      </c>
-      <c r="F58" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -1621,17 +1621,17 @@
       <c r="B59" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D59">
         <v>101</v>
       </c>
-      <c r="D59">
+      <c r="E59">
         <v>83</v>
       </c>
-      <c r="E59">
+      <c r="F59">
         <v>88</v>
-      </c>
-      <c r="F59" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -1641,17 +1641,17 @@
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D60">
         <v>121</v>
       </c>
-      <c r="D60">
+      <c r="E60">
         <v>84</v>
       </c>
-      <c r="E60">
+      <c r="F60">
         <v>89</v>
-      </c>
-      <c r="F60" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -1661,17 +1661,17 @@
       <c r="B61" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D61">
         <v>121</v>
       </c>
-      <c r="D61">
+      <c r="E61">
         <v>85</v>
       </c>
-      <c r="E61">
+      <c r="F61">
         <v>90</v>
-      </c>
-      <c r="F61" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
@@ -1681,17 +1681,17 @@
       <c r="B62" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D62">
         <v>121</v>
       </c>
-      <c r="D62">
+      <c r="E62">
         <v>86</v>
       </c>
-      <c r="E62">
+      <c r="F62">
         <v>91</v>
-      </c>
-      <c r="F62" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
@@ -1701,17 +1701,17 @@
       <c r="B63" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D63">
         <v>121</v>
       </c>
-      <c r="D63">
+      <c r="E63">
         <v>87</v>
       </c>
-      <c r="E63">
+      <c r="F63">
         <v>92</v>
-      </c>
-      <c r="F63" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -1721,17 +1721,17 @@
       <c r="B64" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D64">
         <v>120</v>
       </c>
-      <c r="D64">
+      <c r="E64">
         <v>88</v>
       </c>
-      <c r="E64">
+      <c r="F64">
         <v>93</v>
-      </c>
-      <c r="F64" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
@@ -1741,17 +1741,17 @@
       <c r="B65" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D65">
         <v>120</v>
       </c>
-      <c r="D65">
+      <c r="E65">
         <v>89</v>
       </c>
-      <c r="E65">
+      <c r="F65">
         <v>94</v>
-      </c>
-      <c r="F65" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
@@ -1761,17 +1761,17 @@
       <c r="B66" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D66">
         <v>120</v>
       </c>
-      <c r="D66">
+      <c r="E66">
         <v>90</v>
       </c>
-      <c r="E66">
+      <c r="F66">
         <v>82</v>
-      </c>
-      <c r="F66" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
@@ -1781,17 +1781,17 @@
       <c r="B67" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D67">
         <v>120</v>
       </c>
-      <c r="D67">
+      <c r="E67">
         <v>91</v>
       </c>
-      <c r="E67">
+      <c r="F67">
         <v>71</v>
-      </c>
-      <c r="F67" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
@@ -1801,17 +1801,17 @@
       <c r="B68" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D68">
         <v>120</v>
       </c>
-      <c r="D68">
+      <c r="E68">
         <v>92</v>
       </c>
-      <c r="E68">
+      <c r="F68">
         <v>57</v>
-      </c>
-      <c r="F68" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
@@ -1821,17 +1821,17 @@
       <c r="B69" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D69">
         <v>120</v>
       </c>
-      <c r="D69">
+      <c r="E69">
         <v>93</v>
       </c>
-      <c r="E69">
+      <c r="F69">
         <v>76</v>
-      </c>
-      <c r="F69" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
@@ -1841,17 +1841,17 @@
       <c r="B70" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D70">
         <v>120</v>
       </c>
-      <c r="D70">
+      <c r="E70">
         <v>94</v>
       </c>
-      <c r="E70">
+      <c r="F70">
         <v>65</v>
-      </c>
-      <c r="F70" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
@@ -1861,17 +1861,17 @@
       <c r="B71" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D71">
         <v>120</v>
       </c>
-      <c r="D71">
+      <c r="E71">
         <v>95</v>
       </c>
-      <c r="E71">
+      <c r="F71">
         <v>65</v>
-      </c>
-      <c r="F71" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
@@ -1881,17 +1881,17 @@
       <c r="B72" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D72">
         <v>120</v>
       </c>
-      <c r="D72">
+      <c r="E72">
         <v>96</v>
       </c>
-      <c r="E72">
+      <c r="F72">
         <v>67</v>
-      </c>
-      <c r="F72" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
@@ -1901,17 +1901,17 @@
       <c r="B73" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D73">
         <v>120</v>
       </c>
-      <c r="D73">
+      <c r="E73">
         <v>97</v>
       </c>
-      <c r="E73">
+      <c r="F73">
         <v>69</v>
-      </c>
-      <c r="F73" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
@@ -1921,17 +1921,17 @@
       <c r="B74" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="3">
+        <v>0.41944444444444445</v>
+      </c>
+      <c r="D74">
         <v>120</v>
       </c>
-      <c r="D74">
+      <c r="E74">
         <v>98</v>
       </c>
-      <c r="E74">
+      <c r="F74">
         <v>71</v>
-      </c>
-      <c r="F74" s="3">
-        <v>0.41944444444444445</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
@@ -1941,17 +1941,17 @@
       <c r="B75" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D75">
         <v>111</v>
       </c>
-      <c r="D75">
+      <c r="E75">
         <v>99</v>
       </c>
-      <c r="E75">
+      <c r="F75">
         <v>73</v>
-      </c>
-      <c r="F75" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
@@ -1961,17 +1961,17 @@
       <c r="B76" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D76">
         <v>111</v>
       </c>
-      <c r="D76">
+      <c r="E76">
         <v>100</v>
       </c>
-      <c r="E76">
+      <c r="F76">
         <v>75</v>
-      </c>
-      <c r="F76" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
@@ -1981,17 +1981,17 @@
       <c r="B77" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D77">
         <v>118</v>
       </c>
-      <c r="D77">
+      <c r="E77">
         <v>101</v>
       </c>
-      <c r="E77">
+      <c r="F77">
         <v>77</v>
-      </c>
-      <c r="F77" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
@@ -2001,17 +2001,17 @@
       <c r="B78" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D78">
         <v>108</v>
       </c>
-      <c r="D78">
+      <c r="E78">
         <v>102</v>
       </c>
-      <c r="E78">
+      <c r="F78">
         <v>79</v>
-      </c>
-      <c r="F78" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
@@ -2021,17 +2021,17 @@
       <c r="B79" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D79">
         <v>117</v>
       </c>
-      <c r="D79" s="2">
+      <c r="E79" s="2">
         <v>72</v>
       </c>
-      <c r="E79">
+      <c r="F79">
         <v>81</v>
-      </c>
-      <c r="F79" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
@@ -2041,17 +2041,17 @@
       <c r="B80" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D80">
         <v>126</v>
       </c>
-      <c r="D80" s="2">
+      <c r="E80" s="2">
         <v>72</v>
       </c>
-      <c r="E80">
+      <c r="F80">
         <v>83</v>
-      </c>
-      <c r="F80" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
@@ -2061,17 +2061,17 @@
       <c r="B81" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D81">
         <v>117</v>
       </c>
-      <c r="D81" s="2">
+      <c r="E81" s="2">
         <v>72</v>
       </c>
-      <c r="E81">
+      <c r="F81">
         <v>85</v>
-      </c>
-      <c r="F81" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.35">
@@ -2081,17 +2081,17 @@
       <c r="B82" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D82">
         <v>119</v>
       </c>
-      <c r="D82" s="2">
+      <c r="E82" s="2">
         <v>72</v>
       </c>
-      <c r="E82">
+      <c r="F82">
         <v>87</v>
-      </c>
-      <c r="F82" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
@@ -2101,17 +2101,17 @@
       <c r="B83" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C83">
+      <c r="C83" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D83">
         <v>117</v>
       </c>
-      <c r="D83" s="2">
+      <c r="E83" s="2">
         <v>72</v>
       </c>
-      <c r="E83">
+      <c r="F83">
         <v>89</v>
-      </c>
-      <c r="F83" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
@@ -2121,17 +2121,17 @@
       <c r="B84" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C84">
+      <c r="C84" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D84">
         <v>118</v>
       </c>
-      <c r="D84">
+      <c r="E84">
         <v>75</v>
       </c>
-      <c r="E84">
+      <c r="F84">
         <v>91</v>
-      </c>
-      <c r="F84" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
@@ -2141,17 +2141,17 @@
       <c r="B85" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D85">
         <v>119</v>
       </c>
-      <c r="D85" s="2">
+      <c r="E85" s="2">
         <v>75</v>
       </c>
-      <c r="E85">
+      <c r="F85">
         <v>75</v>
-      </c>
-      <c r="F85" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
@@ -2161,17 +2161,17 @@
       <c r="B86" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C86">
+      <c r="C86" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D86">
         <v>120</v>
       </c>
-      <c r="D86">
+      <c r="E86">
         <v>75</v>
       </c>
-      <c r="E86">
+      <c r="F86">
         <v>64</v>
-      </c>
-      <c r="F86" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
@@ -2181,17 +2181,17 @@
       <c r="B87" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C87">
+      <c r="C87" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D87">
         <v>121</v>
       </c>
-      <c r="D87">
+      <c r="E87">
         <v>76</v>
       </c>
-      <c r="E87">
+      <c r="F87">
         <v>60</v>
-      </c>
-      <c r="F87" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
@@ -2201,17 +2201,17 @@
       <c r="B88" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C88">
+      <c r="C88" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D88">
         <v>122</v>
       </c>
-      <c r="D88">
+      <c r="E88">
         <v>77</v>
       </c>
-      <c r="E88">
+      <c r="F88">
         <v>61</v>
-      </c>
-      <c r="F88" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
@@ -2221,17 +2221,17 @@
       <c r="B89" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D89">
         <v>123</v>
       </c>
-      <c r="D89">
+      <c r="E89">
         <v>78</v>
       </c>
-      <c r="E89">
+      <c r="F89">
         <v>61</v>
-      </c>
-      <c r="F89" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
@@ -2241,17 +2241,17 @@
       <c r="B90" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D90">
         <v>124</v>
       </c>
-      <c r="D90">
+      <c r="E90">
         <v>79</v>
       </c>
-      <c r="E90">
+      <c r="F90">
         <v>61</v>
-      </c>
-      <c r="F90" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
@@ -2261,17 +2261,17 @@
       <c r="B91" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D91">
         <v>125</v>
       </c>
-      <c r="D91">
+      <c r="E91">
         <v>80</v>
       </c>
-      <c r="E91">
+      <c r="F91">
         <v>61</v>
-      </c>
-      <c r="F91" s="3">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
@@ -2281,17 +2281,17 @@
       <c r="B92" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="3">
+        <v>0.39652777777777798</v>
+      </c>
+      <c r="D92">
         <v>126</v>
       </c>
-      <c r="D92">
+      <c r="E92">
         <v>81</v>
       </c>
-      <c r="E92">
+      <c r="F92">
         <v>61</v>
-      </c>
-      <c r="F92" s="3">
-        <v>0.39652777777777798</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
@@ -2301,17 +2301,17 @@
       <c r="B93" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D93">
         <v>127</v>
       </c>
-      <c r="D93">
+      <c r="E93">
         <v>82</v>
       </c>
-      <c r="E93">
+      <c r="F93">
         <v>61</v>
-      </c>
-      <c r="F93" s="3">
-        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>